<commit_message>
INC, DEC, INX, DEX, INY, DEY instructions implementation and tests
</commit_message>
<xml_diff>
--- a/6502_instructions.xlsx
+++ b/6502_instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lukasz\Documents\Projects\VisualStudio\c++\6502_emulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81D6E9C-26EE-4FDD-90F2-CFDDDFE9FEE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44772712-A95F-4E77-917E-B38467B9AF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65254093-C550-4CD0-BC53-E7CEED0B8F89}"/>
   </bookViews>
@@ -587,10 +587,10 @@
     <t>INC abs,X</t>
   </si>
   <si>
-    <t>HIGH BYTE</t>
-  </si>
-  <si>
-    <t>LOW BYTE</t>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>LOW</t>
   </si>
 </sst>
 </file>
@@ -674,9 +674,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -685,6 +682,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1003,7 +1003,7 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,24 +1016,24 @@
       <c r="A1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
     </row>
     <row r="2" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1090,641 +1090,641 @@
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="5" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="5" t="s">
+      <c r="I3" s="3"/>
+      <c r="J3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="5" t="s">
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="4"/>
+      <c r="Q3" s="3"/>
     </row>
     <row r="4" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="5" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="3" t="s">
+      <c r="I4" s="3"/>
+      <c r="J4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="5" t="s">
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="Q4" s="4"/>
+      <c r="Q4" s="3"/>
     </row>
     <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="5" t="s">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="5" t="s">
+      <c r="I5" s="3"/>
+      <c r="J5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="M5" s="4"/>
-      <c r="N5" s="5" t="s">
+      <c r="M5" s="3"/>
+      <c r="N5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="O5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="P5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="Q5" s="4"/>
+      <c r="Q5" s="3"/>
     </row>
     <row r="6" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="5" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="3" t="s">
+      <c r="I6" s="3"/>
+      <c r="J6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="5" t="s">
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="P6" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="Q6" s="4"/>
+      <c r="Q6" s="3"/>
     </row>
     <row r="7" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="5" t="s">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="5" t="s">
+      <c r="I7" s="3"/>
+      <c r="J7" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="M7" s="4"/>
-      <c r="N7" s="5" t="s">
+      <c r="M7" s="3"/>
+      <c r="N7" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="O7" s="5" t="s">
+      <c r="O7" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="P7" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="Q7" s="4"/>
+      <c r="Q7" s="3"/>
     </row>
     <row r="8" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="5" t="s">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="3" t="s">
+      <c r="I8" s="3"/>
+      <c r="J8" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="5" t="s">
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="P8" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="Q8" s="4"/>
+      <c r="Q8" s="3"/>
     </row>
     <row r="9" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="3" t="s">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="5" t="s">
+      <c r="I9" s="3"/>
+      <c r="J9" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="K9" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="L9" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="M9" s="4"/>
-      <c r="N9" s="5" t="s">
+      <c r="M9" s="3"/>
+      <c r="N9" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="O9" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="P9" s="3" t="s">
+      <c r="P9" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="Q9" s="4"/>
+      <c r="Q9" s="3"/>
     </row>
     <row r="10" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="3" t="s">
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="3" t="s">
+      <c r="I10" s="3"/>
+      <c r="J10" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="K10" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="3" t="s">
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="P10" s="3" t="s">
+      <c r="P10" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="Q10" s="4"/>
+      <c r="Q10" s="3"/>
     </row>
     <row r="11" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="5" t="s">
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="3" t="s">
+      <c r="I11" s="3"/>
+      <c r="J11" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="K11" s="4"/>
-      <c r="L11" s="5" t="s">
+      <c r="K11" s="3"/>
+      <c r="L11" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="M11" s="4"/>
-      <c r="N11" s="5" t="s">
+      <c r="M11" s="3"/>
+      <c r="N11" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="O11" s="5" t="s">
+      <c r="O11" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="P11" s="5" t="s">
+      <c r="P11" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="Q11" s="4"/>
+      <c r="Q11" s="3"/>
     </row>
     <row r="12" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="5" t="s">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="5" t="s">
+      <c r="I12" s="3"/>
+      <c r="J12" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="K12" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="L12" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="5" t="s">
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
     </row>
     <row r="13" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="5" t="s">
+      <c r="E13" s="3"/>
+      <c r="F13" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="5" t="s">
+      <c r="I13" s="3"/>
+      <c r="J13" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="K13" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="L13" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="M13" s="4"/>
-      <c r="N13" s="5" t="s">
+      <c r="M13" s="3"/>
+      <c r="N13" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="O13" s="5" t="s">
+      <c r="O13" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="P13" s="5" t="s">
+      <c r="P13" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="Q13" s="4"/>
+      <c r="Q13" s="3"/>
     </row>
     <row r="14" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="5" t="s">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="3" t="s">
+      <c r="I14" s="3"/>
+      <c r="J14" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="K14" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="L14" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="M14" s="4"/>
-      <c r="N14" s="5" t="s">
+      <c r="M14" s="3"/>
+      <c r="N14" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="O14" s="5" t="s">
+      <c r="O14" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="P14" s="5" t="s">
+      <c r="P14" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="Q14" s="4"/>
+      <c r="Q14" s="3"/>
     </row>
     <row r="15" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="3" t="s">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="3" t="s">
+      <c r="I15" s="3"/>
+      <c r="J15" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="K15" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="L15" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="M15" s="4"/>
-      <c r="N15" s="3" t="s">
+      <c r="M15" s="3"/>
+      <c r="N15" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="O15" s="3" t="s">
+      <c r="O15" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="P15" s="3" t="s">
+      <c r="P15" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="Q15" s="4"/>
+      <c r="Q15" s="3"/>
     </row>
     <row r="16" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="3" t="s">
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="I16" s="4"/>
-      <c r="J16" s="3" t="s">
+      <c r="I16" s="3"/>
+      <c r="J16" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="K16" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="3" t="s">
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="P16" s="3" t="s">
+      <c r="P16" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="Q16" s="4"/>
+      <c r="Q16" s="3"/>
     </row>
     <row r="17" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="3" t="s">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="I17" s="4"/>
-      <c r="J17" s="3" t="s">
+      <c r="I17" s="3"/>
+      <c r="J17" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="K17" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="L17" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="M17" s="4"/>
-      <c r="N17" s="3" t="s">
+      <c r="M17" s="3"/>
+      <c r="N17" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="O17" s="3" t="s">
+      <c r="O17" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="P17" s="3" t="s">
+      <c r="P17" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="Q17" s="4"/>
+      <c r="Q17" s="3"/>
     </row>
     <row r="18" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="3" t="s">
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="I18" s="4"/>
-      <c r="J18" s="3" t="s">
+      <c r="I18" s="3"/>
+      <c r="J18" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="K18" s="3" t="s">
+      <c r="K18" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="3" t="s">
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="P18" s="3" t="s">
+      <c r="P18" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="Q18" s="4"/>
+      <c r="Q18" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
tests and implementation:     set status flag:         SEC, SED, SEI     clear status flag:         CLC, CLD, CLI, CLV     branching:         BEQ, BNE, BVC, BVS, BPL, BNE, BCS, BCC     system functions:         NOP
</commit_message>
<xml_diff>
--- a/6502_instructions.xlsx
+++ b/6502_instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lukasz\Documents\Projects\VisualStudio\c++\6502_emulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44772712-A95F-4E77-917E-B38467B9AF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FB75BA-D3DE-49C7-B8A7-6CF76ABFE59D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65254093-C550-4CD0-BC53-E7CEED0B8F89}"/>
   </bookViews>
@@ -1003,7 +1003,7 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,7 +1129,7 @@
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1145,7 +1145,7 @@
         <v>31</v>
       </c>
       <c r="I4" s="3"/>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="4" t="s">
         <v>32</v>
       </c>
       <c r="K4" s="4" t="s">
@@ -1209,7 +1209,7 @@
       <c r="A6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1225,7 +1225,7 @@
         <v>52</v>
       </c>
       <c r="I6" s="3"/>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="4" t="s">
         <v>53</v>
       </c>
       <c r="K6" s="4" t="s">
@@ -1287,7 +1287,7 @@
       <c r="A8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>69</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1303,7 +1303,7 @@
         <v>72</v>
       </c>
       <c r="I8" s="3"/>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="4" t="s">
         <v>73</v>
       </c>
       <c r="K8" s="4" t="s">
@@ -1365,7 +1365,7 @@
       <c r="A10" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>89</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1381,7 +1381,7 @@
         <v>92</v>
       </c>
       <c r="I10" s="3"/>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="4" t="s">
         <v>93</v>
       </c>
       <c r="K10" s="2" t="s">
@@ -1443,7 +1443,7 @@
       <c r="A12" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="4" t="s">
         <v>108</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -1527,7 +1527,7 @@
       <c r="A14" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="4" t="s">
         <v>131</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -1545,7 +1545,7 @@
         <v>135</v>
       </c>
       <c r="I14" s="3"/>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="4" t="s">
         <v>136</v>
       </c>
       <c r="K14" s="4" t="s">
@@ -1584,7 +1584,7 @@
       <c r="G15" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="4" t="s">
         <v>147</v>
       </c>
       <c r="I15" s="3"/>
@@ -1604,7 +1604,7 @@
       <c r="O15" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="P15" s="2" t="s">
+      <c r="P15" s="4" t="s">
         <v>153</v>
       </c>
       <c r="Q15" s="3"/>
@@ -1613,7 +1613,7 @@
       <c r="A16" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="4" t="s">
         <v>155</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -1625,11 +1625,11 @@
       <c r="G16" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="4" t="s">
         <v>158</v>
       </c>
       <c r="I16" s="3"/>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="4" t="s">
         <v>159</v>
       </c>
       <c r="K16" s="2" t="s">
@@ -1641,7 +1641,7 @@
       <c r="O16" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="P16" s="2" t="s">
+      <c r="P16" s="4" t="s">
         <v>162</v>
       </c>
       <c r="Q16" s="3"/>
@@ -1664,7 +1664,7 @@
       <c r="G17" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="4" t="s">
         <v>168</v>
       </c>
       <c r="I17" s="3"/>
@@ -1674,7 +1674,7 @@
       <c r="K17" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="L17" s="4" t="s">
         <v>171</v>
       </c>
       <c r="M17" s="3"/>
@@ -1684,7 +1684,7 @@
       <c r="O17" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="P17" s="2" t="s">
+      <c r="P17" s="4" t="s">
         <v>174</v>
       </c>
       <c r="Q17" s="3"/>
@@ -1693,7 +1693,7 @@
       <c r="A18" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="4" t="s">
         <v>176</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -1705,11 +1705,11 @@
       <c r="G18" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="4" t="s">
         <v>179</v>
       </c>
       <c r="I18" s="3"/>
-      <c r="J18" s="2" t="s">
+      <c r="J18" s="4" t="s">
         <v>180</v>
       </c>
       <c r="K18" s="2" t="s">
@@ -1721,7 +1721,7 @@
       <c r="O18" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="P18" s="2" t="s">
+      <c r="P18" s="4" t="s">
         <v>183</v>
       </c>
       <c r="Q18" s="3"/>

</xml_diff>

<commit_message>
tests and implementation for   ADC, CMP, CPX, CPY
</commit_message>
<xml_diff>
--- a/6502_instructions.xlsx
+++ b/6502_instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lukasz\Documents\Projects\VisualStudio\c++\6502_emulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FB75BA-D3DE-49C7-B8A7-6CF76ABFE59D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23474D9B-5427-444B-9F97-BE54C4DCDCA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65254093-C550-4CD0-BC53-E7CEED0B8F89}"/>
   </bookViews>
@@ -1003,7 +1003,7 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB10" sqref="AB10"/>
+      <selection activeCell="P9" sqref="P8:P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,13 +1327,13 @@
       <c r="B9" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="4" t="s">
         <v>79</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="4" t="s">
         <v>80</v>
       </c>
       <c r="H9" s="2" t="s">
@@ -1343,7 +1343,7 @@
       <c r="J9" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="4" t="s">
         <v>83</v>
       </c>
       <c r="L9" s="2" t="s">
@@ -1353,7 +1353,7 @@
       <c r="N9" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="O9" s="4" t="s">
         <v>86</v>
       </c>
       <c r="P9" s="2" t="s">
@@ -1368,13 +1368,13 @@
       <c r="B10" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="4" t="s">
         <v>90</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="4" t="s">
         <v>91</v>
       </c>
       <c r="H10" s="2" t="s">
@@ -1384,13 +1384,13 @@
       <c r="J10" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="4" t="s">
         <v>94</v>
       </c>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
-      <c r="O10" s="2" t="s">
+      <c r="O10" s="4" t="s">
         <v>95</v>
       </c>
       <c r="P10" s="2" t="s">

</xml_diff>

<commit_message>
start implementing SBC (fail tests)
</commit_message>
<xml_diff>
--- a/6502_instructions.xlsx
+++ b/6502_instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lukasz\Documents\Projects\VisualStudio\c++\6502_emulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23474D9B-5427-444B-9F97-BE54C4DCDCA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACDDE402-5728-44D4-9FE3-CE4F7BD92C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65254093-C550-4CD0-BC53-E7CEED0B8F89}"/>
   </bookViews>
@@ -1003,7 +1003,7 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P9" sqref="P8:P9"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1570,18 +1570,18 @@
       <c r="A15" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="4" t="s">
         <v>144</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="4" t="s">
         <v>146</v>
       </c>
       <c r="H15" s="4" t="s">
@@ -1591,17 +1591,17 @@
       <c r="J15" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K15" s="4" t="s">
         <v>149</v>
       </c>
       <c r="L15" s="4" t="s">
         <v>150</v>
       </c>
       <c r="M15" s="3"/>
-      <c r="N15" s="2" t="s">
+      <c r="N15" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="O15" s="2" t="s">
+      <c r="O15" s="4" t="s">
         <v>152</v>
       </c>
       <c r="P15" s="4" t="s">
@@ -1616,13 +1616,13 @@
       <c r="B16" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="4" t="s">
         <v>156</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="4" t="s">
         <v>157</v>
       </c>
       <c r="H16" s="4" t="s">
@@ -1632,13 +1632,13 @@
       <c r="J16" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="K16" s="4" t="s">
         <v>160</v>
       </c>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
-      <c r="O16" s="2" t="s">
+      <c r="O16" s="4" t="s">
         <v>161</v>
       </c>
       <c r="P16" s="4" t="s">
@@ -1650,7 +1650,7 @@
       <c r="A17" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="4" t="s">
         <v>164</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1658,7 +1658,7 @@
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="4" t="s">
         <v>166</v>
       </c>
       <c r="G17" s="2" t="s">
@@ -1678,7 +1678,7 @@
         <v>171</v>
       </c>
       <c r="M17" s="3"/>
-      <c r="N17" s="2" t="s">
+      <c r="N17" s="4" t="s">
         <v>172</v>
       </c>
       <c r="O17" s="2" t="s">

</xml_diff>

<commit_message>
update instructions excel sheet
</commit_message>
<xml_diff>
--- a/6502_instructions.xlsx
+++ b/6502_instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lukasz\Documents\Projects\VisualStudio\c++\6502_emulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACDDE402-5728-44D4-9FE3-CE4F7BD92C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C120F150-B1F3-4D81-B582-09FBE35CFA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65254093-C550-4CD0-BC53-E7CEED0B8F89}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="185">
   <si>
     <t>‐0</t>
   </si>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t>ORA X,ind</t>
-  </si>
-  <si>
-    <t>---</t>
   </si>
   <si>
     <t>ORA zpg</t>
@@ -1003,7 +1000,7 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1014,10 +1011,10 @@
   <sheetData>
     <row r="1" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>184</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>185</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -1100,629 +1097,627 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="L3" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="Q3" s="3"/>
     </row>
     <row r="4" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="Q4" s="3"/>
     </row>
     <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="L5" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="M5" s="3"/>
       <c r="N5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="O5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="P5" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="Q5" s="3"/>
     </row>
     <row r="6" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="P6" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="Q6" s="3"/>
     </row>
     <row r="7" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="L7" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="M7" s="3"/>
       <c r="N7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="O7" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="O7" s="4" t="s">
+      <c r="P7" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="Q7" s="3"/>
     </row>
     <row r="8" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K8" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="P8" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="Q8" s="3"/>
     </row>
     <row r="9" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K9" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="L9" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="M9" s="3"/>
       <c r="N9" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="O9" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="O9" s="4" t="s">
+      <c r="P9" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="Q9" s="3"/>
     </row>
     <row r="10" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="K10" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="P10" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="Q10" s="3"/>
     </row>
     <row r="11" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>100</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>101</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K11" s="3"/>
       <c r="L11" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M11" s="3"/>
       <c r="N11" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="O11" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="O11" s="4" t="s">
+      <c r="P11" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="Q11" s="3"/>
     </row>
     <row r="12" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>108</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>109</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="H12" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>112</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K12" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="L12" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
     </row>
     <row r="13" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>120</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>122</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>123</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K13" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="L13" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>126</v>
       </c>
       <c r="M13" s="3"/>
       <c r="N13" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="O13" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="O13" s="4" t="s">
+      <c r="P13" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="P13" s="4" t="s">
-        <v>129</v>
       </c>
       <c r="Q13" s="3"/>
     </row>
     <row r="14" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>132</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>134</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>135</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="K14" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="L14" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>138</v>
       </c>
       <c r="M14" s="3"/>
       <c r="N14" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="O14" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="O14" s="4" t="s">
+      <c r="P14" s="4" t="s">
         <v>140</v>
-      </c>
-      <c r="P14" s="4" t="s">
-        <v>141</v>
       </c>
       <c r="Q14" s="3"/>
     </row>
     <row r="15" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>144</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="H15" s="4" t="s">
         <v>146</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>147</v>
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="K15" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="L15" s="4" t="s">
         <v>149</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>150</v>
       </c>
       <c r="M15" s="3"/>
       <c r="N15" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="O15" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="O15" s="4" t="s">
+      <c r="P15" s="4" t="s">
         <v>152</v>
-      </c>
-      <c r="P15" s="4" t="s">
-        <v>153</v>
       </c>
       <c r="Q15" s="3"/>
     </row>
     <row r="16" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>155</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>156</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="H16" s="4" t="s">
         <v>157</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>158</v>
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="K16" s="4" t="s">
         <v>159</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>160</v>
       </c>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
       <c r="O16" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="P16" s="4" t="s">
         <v>161</v>
-      </c>
-      <c r="P16" s="4" t="s">
-        <v>162</v>
       </c>
       <c r="Q16" s="3"/>
     </row>
     <row r="17" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>164</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>165</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="H17" s="4" t="s">
         <v>167</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>168</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="K17" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="L17" s="4" t="s">
         <v>170</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>171</v>
       </c>
       <c r="M17" s="3"/>
       <c r="N17" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="O17" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="O17" s="2" t="s">
+      <c r="P17" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="P17" s="4" t="s">
-        <v>174</v>
       </c>
       <c r="Q17" s="3"/>
     </row>
     <row r="18" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>176</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>177</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="H18" s="4" t="s">
         <v>178</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>179</v>
       </c>
       <c r="I18" s="3"/>
       <c r="J18" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="K18" s="4" t="s">
         <v>180</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>181</v>
       </c>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
-      <c r="O18" s="2" t="s">
+      <c r="O18" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="P18" s="4" t="s">
         <v>182</v>
-      </c>
-      <c r="P18" s="4" t="s">
-        <v>183</v>
       </c>
       <c r="Q18" s="3"/>
     </row>

</xml_diff>

<commit_message>
ASL and LSR implementation and tests
</commit_message>
<xml_diff>
--- a/6502_instructions.xlsx
+++ b/6502_instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lukasz\Documents\Projects\VisualStudio\c++\6502_emulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C120F150-B1F3-4D81-B582-09FBE35CFA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7238390-355D-4AF0-819D-AEB236C724BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65254093-C550-4CD0-BC53-E7CEED0B8F89}"/>
   </bookViews>
@@ -1000,7 +1000,7 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1099,7 +1099,7 @@
       <c r="G3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I3" s="3"/>
@@ -1109,7 +1109,7 @@
       <c r="K3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="4" t="s">
         <v>23</v>
       </c>
       <c r="M3" s="3"/>
@@ -1117,7 +1117,7 @@
       <c r="O3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="P3" s="4" t="s">
         <v>25</v>
       </c>
       <c r="Q3" s="3"/>
@@ -1138,7 +1138,7 @@
       <c r="G4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="4" t="s">
         <v>30</v>
       </c>
       <c r="I4" s="3"/>
@@ -1154,7 +1154,7 @@
       <c r="O4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="P4" s="4" t="s">
         <v>34</v>
       </c>
       <c r="Q4" s="3"/>
@@ -1255,7 +1255,7 @@
       <c r="G7" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="4" t="s">
         <v>60</v>
       </c>
       <c r="I7" s="3"/>
@@ -1265,7 +1265,7 @@
       <c r="K7" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="4" t="s">
         <v>63</v>
       </c>
       <c r="M7" s="3"/>
@@ -1275,7 +1275,7 @@
       <c r="O7" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="P7" s="4" t="s">
         <v>66</v>
       </c>
       <c r="Q7" s="3"/>
@@ -1296,7 +1296,7 @@
       <c r="G8" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="4" t="s">
         <v>71</v>
       </c>
       <c r="I8" s="3"/>
@@ -1312,7 +1312,7 @@
       <c r="O8" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="P8" s="4" t="s">
         <v>75</v>
       </c>
       <c r="Q8" s="3"/>

</xml_diff>

<commit_message>
ROL and ROR implementation and tests
</commit_message>
<xml_diff>
--- a/6502_instructions.xlsx
+++ b/6502_instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lukasz\Documents\Projects\VisualStudio\c++\6502_emulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7238390-355D-4AF0-819D-AEB236C724BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54B1B66-AF57-43C0-AE4A-61F4A2604157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65254093-C550-4CD0-BC53-E7CEED0B8F89}"/>
   </bookViews>
@@ -1000,7 +1000,7 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,7 +1177,7 @@
       <c r="G5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="4" t="s">
         <v>40</v>
       </c>
       <c r="I5" s="3"/>
@@ -1187,7 +1187,7 @@
       <c r="K5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="4" t="s">
         <v>43</v>
       </c>
       <c r="M5" s="3"/>
@@ -1197,7 +1197,7 @@
       <c r="O5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="P5" s="4" t="s">
         <v>46</v>
       </c>
       <c r="Q5" s="3"/>
@@ -1218,7 +1218,7 @@
       <c r="G6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="4" t="s">
         <v>51</v>
       </c>
       <c r="I6" s="3"/>
@@ -1234,7 +1234,7 @@
       <c r="O6" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="P6" s="4" t="s">
         <v>55</v>
       </c>
       <c r="Q6" s="3"/>
@@ -1333,7 +1333,7 @@
       <c r="G9" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="4" t="s">
         <v>80</v>
       </c>
       <c r="I9" s="3"/>
@@ -1343,7 +1343,7 @@
       <c r="K9" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="L9" s="4" t="s">
         <v>83</v>
       </c>
       <c r="M9" s="3"/>
@@ -1353,7 +1353,7 @@
       <c r="O9" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="P9" s="2" t="s">
+      <c r="P9" s="4" t="s">
         <v>86</v>
       </c>
       <c r="Q9" s="3"/>
@@ -1374,7 +1374,7 @@
       <c r="G10" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="4" t="s">
         <v>91</v>
       </c>
       <c r="I10" s="3"/>
@@ -1390,7 +1390,7 @@
       <c r="O10" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="P10" s="2" t="s">
+      <c r="P10" s="4" t="s">
         <v>95</v>
       </c>
       <c r="Q10" s="3"/>

</xml_diff>

<commit_message>
implement BRK and RTI, FIX Branching cycles count FIX wraparound in Indirect X addressing mode, FIX flags in PHP, PLP, add test with program that tests all the instructions
</commit_message>
<xml_diff>
--- a/6502_instructions.xlsx
+++ b/6502_instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lukasz\Documents\Projects\VisualStudio\c++\6502_emulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54B1B66-AF57-43C0-AE4A-61F4A2604157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40621BBA-4791-4286-ADCB-B23DFD597C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65254093-C550-4CD0-BC53-E7CEED0B8F89}"/>
   </bookViews>
@@ -666,13 +666,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1000,7 +997,7 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,24 +1010,24 @@
       <c r="A1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
     </row>
     <row r="2" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1087,639 +1084,639 @@
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="4" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="4" t="s">
+      <c r="I3" s="2"/>
+      <c r="J3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="4" t="s">
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="Q3" s="3"/>
+      <c r="Q3" s="2"/>
     </row>
     <row r="4" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="4" t="s">
+      <c r="I4" s="2"/>
+      <c r="J4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="4" t="s">
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="P4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="Q4" s="3"/>
+      <c r="Q4" s="2"/>
     </row>
     <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="4" t="s">
+      <c r="I5" s="2"/>
+      <c r="J5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="M5" s="3"/>
-      <c r="N5" s="4" t="s">
+      <c r="M5" s="2"/>
+      <c r="N5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="P5" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="Q5" s="3"/>
+      <c r="Q5" s="2"/>
     </row>
     <row r="6" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="4" t="s">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="4" t="s">
+      <c r="I6" s="2"/>
+      <c r="J6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="4" t="s">
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="P6" s="4" t="s">
+      <c r="P6" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Q6" s="3"/>
+      <c r="Q6" s="2"/>
     </row>
     <row r="7" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4" t="s">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="4" t="s">
+      <c r="I7" s="2"/>
+      <c r="J7" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="M7" s="3"/>
-      <c r="N7" s="4" t="s">
+      <c r="M7" s="2"/>
+      <c r="N7" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="O7" s="4" t="s">
+      <c r="O7" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="P7" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="Q7" s="3"/>
+      <c r="Q7" s="2"/>
     </row>
     <row r="8" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="4" t="s">
+      <c r="I8" s="2"/>
+      <c r="J8" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="4" t="s">
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="P8" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="Q8" s="3"/>
+      <c r="Q8" s="2"/>
     </row>
     <row r="9" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="4" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="4" t="s">
+      <c r="I9" s="2"/>
+      <c r="J9" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="M9" s="3"/>
-      <c r="N9" s="4" t="s">
+      <c r="M9" s="2"/>
+      <c r="N9" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="O9" s="4" t="s">
+      <c r="O9" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="P9" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="Q9" s="3"/>
+      <c r="Q9" s="2"/>
     </row>
     <row r="10" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="4" t="s">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="4" t="s">
+      <c r="I10" s="2"/>
+      <c r="J10" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="4" t="s">
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="P10" s="4" t="s">
+      <c r="P10" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="Q10" s="3"/>
+      <c r="Q10" s="2"/>
     </row>
     <row r="11" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="4" t="s">
+      <c r="I11" s="2"/>
+      <c r="J11" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="K11" s="3"/>
-      <c r="L11" s="4" t="s">
+      <c r="K11" s="2"/>
+      <c r="L11" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="M11" s="3"/>
-      <c r="N11" s="4" t="s">
+      <c r="M11" s="2"/>
+      <c r="N11" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="O11" s="4" t="s">
+      <c r="O11" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="P11" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="Q11" s="3"/>
+      <c r="Q11" s="2"/>
     </row>
     <row r="12" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="4" t="s">
+      <c r="I12" s="2"/>
+      <c r="J12" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="L12" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="4" t="s">
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
     </row>
     <row r="13" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4" t="s">
+      <c r="E13" s="2"/>
+      <c r="F13" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="4" t="s">
+      <c r="I13" s="2"/>
+      <c r="J13" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="K13" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="L13" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="M13" s="3"/>
-      <c r="N13" s="4" t="s">
+      <c r="M13" s="2"/>
+      <c r="N13" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="O13" s="4" t="s">
+      <c r="O13" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="P13" s="4" t="s">
+      <c r="P13" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="Q13" s="3"/>
+      <c r="Q13" s="2"/>
     </row>
     <row r="14" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="4" t="s">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="4" t="s">
+      <c r="I14" s="2"/>
+      <c r="J14" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="L14" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="M14" s="3"/>
-      <c r="N14" s="4" t="s">
+      <c r="M14" s="2"/>
+      <c r="N14" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="O14" s="4" t="s">
+      <c r="O14" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="P14" s="4" t="s">
+      <c r="P14" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="Q14" s="3"/>
+      <c r="Q14" s="2"/>
     </row>
     <row r="15" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="4" t="s">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="I15" s="3"/>
-      <c r="J15" s="4" t="s">
+      <c r="I15" s="2"/>
+      <c r="J15" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="L15" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="M15" s="3"/>
-      <c r="N15" s="4" t="s">
+      <c r="M15" s="2"/>
+      <c r="N15" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="O15" s="4" t="s">
+      <c r="O15" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="P15" s="4" t="s">
+      <c r="P15" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="Q15" s="3"/>
+      <c r="Q15" s="2"/>
     </row>
     <row r="16" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="4" t="s">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="4" t="s">
+      <c r="I16" s="2"/>
+      <c r="J16" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="K16" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="4" t="s">
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="P16" s="4" t="s">
+      <c r="P16" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="Q16" s="3"/>
+      <c r="Q16" s="2"/>
     </row>
     <row r="17" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="4" t="s">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="4" t="s">
+      <c r="I17" s="2"/>
+      <c r="J17" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="L17" s="4" t="s">
+      <c r="L17" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="M17" s="3"/>
-      <c r="N17" s="4" t="s">
+      <c r="M17" s="2"/>
+      <c r="N17" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="O17" s="4" t="s">
+      <c r="O17" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="P17" s="4" t="s">
+      <c r="P17" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="Q17" s="3"/>
+      <c r="Q17" s="2"/>
     </row>
     <row r="18" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="4" t="s">
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="4" t="s">
+      <c r="I18" s="2"/>
+      <c r="J18" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="K18" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="4" t="s">
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="P18" s="4" t="s">
+      <c r="P18" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="Q18" s="3"/>
+      <c r="Q18" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>